<commit_message>
Switched to new class data
</commit_message>
<xml_diff>
--- a/public/New_Class_Data.xlsx
+++ b/public/New_Class_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CJ\Documents\My Projects\React_Practice\talium-schedule\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CJ\Documents\My Projects\React_Practice\talium-class-finder\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D996DF56-D577-4311-8A85-EE74911B73FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3BEFDA-CCC2-410E-9DC2-44CCF3687B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Blue | Purple | Red | Brown | Jr Black</t>
-  </si>
-  <si>
     <t>SWAT Demo Team</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Friday</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Black: 1 Dan | Black: 2 Dan</t>
   </si>
   <si>
@@ -128,10 +122,10 @@
     <t>Day_Number</t>
   </si>
   <si>
-    <t>No Belt | White | Yellow | Orange</t>
-  </si>
-  <si>
     <t>No | White | Yellow</t>
+  </si>
+  <si>
+    <t>Purple | Red | Brown | (Children/Teen)</t>
   </si>
 </sst>
 </file>
@@ -198,10 +192,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7017218-20EE-44E7-9F4F-FA44F9F6F436}" name="Table1" displayName="Table1" ref="A1:H48" totalsRowShown="0">
-  <autoFilter ref="A1:H48" xr:uid="{E7017218-20EE-44E7-9F4F-FA44F9F6F436}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H48">
-    <sortCondition ref="E1:E48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7017218-20EE-44E7-9F4F-FA44F9F6F436}" name="Table1" displayName="Table1" ref="A1:H43" totalsRowShown="0">
+  <autoFilter ref="A1:H43" xr:uid="{E7017218-20EE-44E7-9F4F-FA44F9F6F436}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H43">
+    <sortCondition ref="E1:E43"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{364E8D2B-CEB4-44E0-AA92-44857CDDF2E8}" name="ID">
@@ -482,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -507,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -521,7 +515,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f t="shared" ref="A2:A48" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A43" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -549,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -564,7 +558,7 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -597,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -606,10 +600,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="G5" s="1">
-        <v>0.70486111111111116</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -621,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -630,10 +624,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="G6" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
@@ -645,7 +639,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -654,13 +648,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="G7" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -669,7 +663,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -678,13 +672,13 @@
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="G8" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -693,22 +687,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.65625</v>
       </c>
       <c r="G9" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="H9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -717,7 +711,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -726,13 +720,13 @@
         <v>2</v>
       </c>
       <c r="F10" s="1">
-        <v>0.65625</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="G10" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -741,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -750,13 +744,13 @@
         <v>2</v>
       </c>
       <c r="F11" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="G11" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -765,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -774,10 +768,10 @@
         <v>2</v>
       </c>
       <c r="F12" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="G12" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="H12" t="s">
         <v>7</v>
@@ -789,7 +783,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -801,10 +795,10 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="G13" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="H13" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -813,7 +807,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -822,13 +816,13 @@
         <v>2</v>
       </c>
       <c r="F14" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="G14" s="1">
-        <v>0.76041666666666663</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -837,7 +831,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -846,13 +840,13 @@
         <v>2</v>
       </c>
       <c r="F15" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="G15" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="H15" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -870,10 +864,10 @@
         <v>2</v>
       </c>
       <c r="F16" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="G16" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.86111111111111116</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -888,19 +882,19 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.65625</v>
       </c>
       <c r="G17" s="1">
-        <v>0.82291666666666663</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -909,22 +903,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1">
-        <v>0.82291666666666663</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="G18" s="1">
-        <v>0.86111111111111116</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="H18" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -933,7 +927,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -942,13 +936,13 @@
         <v>3</v>
       </c>
       <c r="F19" s="1">
-        <v>0.65625</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="G19" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="H19" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -957,7 +951,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -966,13 +960,13 @@
         <v>3</v>
       </c>
       <c r="F20" s="1">
-        <v>0.67361111111111116</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="G20" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="H20" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -981,7 +975,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -990,10 +984,10 @@
         <v>3</v>
       </c>
       <c r="F21" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="G21" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="H21" t="s">
         <v>7</v>
@@ -1005,7 +999,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -1014,13 +1008,13 @@
         <v>3</v>
       </c>
       <c r="F22" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="G22" s="1">
-        <v>0.70486111111111116</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="H22" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1029,7 +1023,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -1038,13 +1032,13 @@
         <v>3</v>
       </c>
       <c r="F23" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="G23" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="H23" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1053,7 +1047,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1062,13 +1056,13 @@
         <v>3</v>
       </c>
       <c r="F24" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="G24" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.78819444444444442</v>
       </c>
       <c r="H24" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1077,7 +1071,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -1086,13 +1080,13 @@
         <v>3</v>
       </c>
       <c r="F25" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="G25" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1101,7 +1095,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1110,13 +1104,13 @@
         <v>3</v>
       </c>
       <c r="F26" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G26" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.87152777777777779</v>
       </c>
       <c r="H26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1125,7 +1119,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1134,13 +1128,13 @@
         <v>3</v>
       </c>
       <c r="F27" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G27" s="1">
-        <v>0.78819444444444442</v>
+        <v>0.87152777777777779</v>
       </c>
       <c r="H27" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1149,22 +1143,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F28" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.65625</v>
       </c>
       <c r="G28" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="H28" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1173,19 +1167,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.65625</v>
       </c>
       <c r="G29" s="1">
-        <v>0.87152777777777779</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="H29" t="s">
         <v>7</v>
@@ -1197,22 +1191,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="G30" s="1">
-        <v>0.87152777777777779</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="H30" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1221,7 +1215,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
         <v>20</v>
@@ -1230,10 +1224,10 @@
         <v>4</v>
       </c>
       <c r="F31" s="1">
-        <v>0.65625</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="G31" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="H31" t="s">
         <v>7</v>
@@ -1245,7 +1239,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
         <v>20</v>
@@ -1254,10 +1248,10 @@
         <v>4</v>
       </c>
       <c r="F32" s="1">
-        <v>0.65625</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="G32" s="1">
-        <v>0.67708333333333337</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="H32" t="s">
         <v>7</v>
@@ -1269,7 +1263,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>
@@ -1278,10 +1272,10 @@
         <v>4</v>
       </c>
       <c r="F33" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="G33" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="H33" t="s">
         <v>7</v>
@@ -1293,7 +1287,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
         <v>20</v>
@@ -1302,13 +1296,13 @@
         <v>4</v>
       </c>
       <c r="F34" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="G34" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="H34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1317,7 +1311,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
         <v>20</v>
@@ -1326,13 +1320,13 @@
         <v>4</v>
       </c>
       <c r="F35" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="G35" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.86111111111111116</v>
       </c>
       <c r="H35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1341,19 +1335,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F36" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.65625</v>
       </c>
       <c r="G36" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="H36" t="s">
         <v>7</v>
@@ -1368,16 +1362,16 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F37" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="G37" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="H37" t="s">
         <v>7</v>
@@ -1392,19 +1386,19 @@
         <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F38" s="1">
-        <v>0.76736111111111116</v>
+        <v>0.71180555555555558</v>
       </c>
       <c r="G38" s="1">
-        <v>0.79513888888888884</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="H38" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1413,19 +1407,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F39" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G39" s="1">
         <v>0.76736111111111116</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0.79513888888888884</v>
       </c>
       <c r="H39" t="s">
         <v>7</v>
@@ -1433,26 +1427,26 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F40" s="1">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="G40" s="1">
         <v>0.79513888888888884</v>
       </c>
-      <c r="G40" s="1">
-        <v>0.82291666666666663</v>
-      </c>
       <c r="H40" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1461,22 +1455,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F41" s="1">
-        <v>0.82291666666666663</v>
+        <v>0.76736111111111116</v>
       </c>
       <c r="G41" s="1">
-        <v>0.86111111111111116</v>
+        <v>0.78819444444444442</v>
       </c>
       <c r="H41" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1485,22 +1479,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E42">
         <v>5</v>
       </c>
       <c r="F42" s="1">
-        <v>0.65625</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="G42" s="1">
-        <v>0.67708333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H42" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1509,141 +1503,21 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E43">
         <v>5</v>
       </c>
       <c r="F43" s="1">
-        <v>0.68402777777777779</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="G43" s="1">
-        <v>0.71180555555555558</v>
+        <v>0.84375</v>
       </c>
       <c r="H43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44">
-        <v>5</v>
-      </c>
-      <c r="F44" s="1">
-        <v>0.71180555555555558</v>
-      </c>
-      <c r="G44" s="1">
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="H44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" t="s">
-        <v>24</v>
-      </c>
-      <c r="E45">
-        <v>5</v>
-      </c>
-      <c r="F45" s="1">
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="G45" s="1">
-        <v>0.76736111111111116</v>
-      </c>
-      <c r="H45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46">
-        <v>5</v>
-      </c>
-      <c r="F46" s="1">
-        <v>0.76736111111111116</v>
-      </c>
-      <c r="G46" s="1">
-        <v>0.78819444444444442</v>
-      </c>
-      <c r="H46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47">
-        <v>5</v>
-      </c>
-      <c r="F47" s="1">
-        <v>0.79513888888888884</v>
-      </c>
-      <c r="G47" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="H47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48">
-        <v>5</v>
-      </c>
-      <c r="F48" s="1">
-        <v>0.79513888888888884</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0.84375</v>
-      </c>
-      <c r="H48" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>